<commit_message>
Main Assignment 100% Done
</commit_message>
<xml_diff>
--- a/Rest Assured/Main_Assignment_Rest_Assured/src/test/resources/Details.xlsx
+++ b/Rest Assured/Main_Assignment_Rest_Assured/src/test/resources/Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\API TRACK\Rest Assured\Main_Assignment_Rest_Assured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144B64CB-89F3-4920-8C6F-D42E7F90FC01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923BB98A-4B3E-4F62-8B11-4F9D987D7FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{53CBE4F2-3482-48BE-8AE9-252EBD96A7D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{53CBE4F2-3482-48BE-8AE9-252EBD96A7D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Yash Mittal</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Investing</t>
+  </si>
+  <si>
+    <t>yog@deloitte.com</t>
+  </si>
+  <si>
+    <t>yogi@up1</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514A9FF1-540C-42B0-B466-62C71A843DF2}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,16 +586,22 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{0C68079F-E5CD-4D4C-83DC-43F649F96F20}"/>
     <hyperlink ref="B2" r:id="rId2" display="mittal@1" xr:uid="{710D424C-6A1F-4087-B4CB-F0F79CF7AF05}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{A52EE909-BCF7-4B73-8B2A-E54CF71955B1}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{32C13A19-27CE-4AF9-89AF-4B182BEFA75F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -597,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B7D54BF-E7E1-4725-8018-5619D04E500B}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Committing because of alert message given by git guardian
</commit_message>
<xml_diff>
--- a/Rest Assured/Main_Assignment_Rest_Assured/src/test/resources/Details.xlsx
+++ b/Rest Assured/Main_Assignment_Rest_Assured/src/test/resources/Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashmittal2\Desktop\API TRACK\Rest Assured\Main_Assignment_Rest_Assured\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923BB98A-4B3E-4F62-8B11-4F9D987D7FA9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD266372-4A4D-4E4A-8567-F9CB5CA06762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{53CBE4F2-3482-48BE-8AE9-252EBD96A7D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53CBE4F2-3482-48BE-8AE9-252EBD96A7D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Yash Mittal</t>
   </si>
   <si>
-    <t>mittal@2</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Video Chat with Friends</t>
   </si>
   <si>
-    <t>ymittal2@deloitte.com</t>
-  </si>
-  <si>
     <t>Watching Shark tank</t>
   </si>
   <si>
@@ -126,10 +120,16 @@
     <t>Investing</t>
   </si>
   <si>
-    <t>yog@deloitte.com</t>
-  </si>
-  <si>
     <t>yogi@up1</t>
+  </si>
+  <si>
+    <t>mittal@3</t>
+  </si>
+  <si>
+    <t>ymittal3@com</t>
+  </si>
+  <si>
+    <t>yog@com</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2DE8CA-BC64-4DEC-BC96-FBDC735F7224}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,16 +514,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -531,10 +531,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="D2">
         <v>21</v>
@@ -548,7 +548,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6F13488D-3A3A-44AB-BBB1-BBBF5D866E99}"/>
-    <hyperlink ref="C2" r:id="rId2" display="mittal@1" xr:uid="{CC338259-FE90-4ACE-9391-68801F8538EE}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{CC338259-FE90-4ACE-9391-68801F8538EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -559,44 +559,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514A9FF1-540C-42B0-B466-62C71A843DF2}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
     <col min="2" max="2" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{0C68079F-E5CD-4D4C-83DC-43F649F96F20}"/>
-    <hyperlink ref="B2" r:id="rId2" display="mittal@1" xr:uid="{710D424C-6A1F-4087-B4CB-F0F79CF7AF05}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{710D424C-6A1F-4087-B4CB-F0F79CF7AF05}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{A52EE909-BCF7-4B73-8B2A-E54CF71955B1}"/>
     <hyperlink ref="B3" r:id="rId4" xr:uid="{32C13A19-27CE-4AF9-89AF-4B182BEFA75F}"/>
   </hyperlinks>
@@ -620,107 +620,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -744,15 +744,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>4.1666666666666664E-2</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
         <v>4.2361111111111106E-2</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
         <v>8.4027777777777798E-2</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>0.125694444444444</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>0.16736111111111099</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>0.20902777777777801</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2">
         <v>0.250694444444444</v>
@@ -808,7 +808,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2">
         <v>0.29236111111111102</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>0.33402777777777798</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>0.375694444444444</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>0.41736111111111102</v>
@@ -840,7 +840,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>0.45902777777777798</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="2">
         <v>0.500694444444444</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>0.54236111111111096</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>0.58402777777777803</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>0.625694444444444</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>0.66736111111111096</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <v>0.70902777777777803</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>0.750694444444444</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2">
         <v>0.79236111111111096</v>

</xml_diff>